<commit_message>
Auto crwaler fund price for xlsx worksheet
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,21 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" filterPrivacy="true"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D3EC8-FD61-DB48-9E85-C4BF46FD3B57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="72000" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="501029" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>501029 华宝红利</t>
+  </si>
+  <si>
+    <t>金额</t>
+  </si>
+  <si>
+    <t>份额</t>
+  </si>
+  <si>
+    <t>100032 富国中证红利</t>
+  </si>
+  <si>
+    <t>001052 华夏中证500ETF</t>
+  </si>
+  <si>
+    <t>001051 华夏上证50ETF</t>
+  </si>
+  <si>
+    <t>501050 华夏上证50AH</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="165" formatCode="[$¥-804]#,##0.00"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,14 +72,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -376,41 +413,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A6:D6"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="C1" t="str">
-        <v>501029 华宝红利</v>
-      </c>
-      <c r="D1" t="str">
-        <v>金额</v>
-      </c>
-      <c r="E1" t="str">
-        <v>份额</v>
-      </c>
-      <c r="G1" t="str">
-        <v>100032 富国中证红利</v>
-      </c>
-      <c r="K1" t="str">
-        <v>001052 华夏中证500ETF</v>
-      </c>
-      <c r="O1" t="str">
-        <v>001051 华夏上证50ETF</v>
-      </c>
-      <c r="S1" t="str">
-        <v>501050 华夏上证50AH</v>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>43292</v>
       </c>
       <c r="C2">
-        <v>0.9301</v>
+        <v>0.93010000000000004</v>
       </c>
       <c r="D2">
         <v>-2000</v>
@@ -428,7 +468,7 @@
         <v>1954.01</v>
       </c>
       <c r="K2">
-        <v>0.549</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="L2">
         <v>-3000</v>
@@ -437,7 +477,7 @@
         <v>5457.92</v>
       </c>
       <c r="O2">
-        <v>0.833</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="P2">
         <v>-3000</v>
@@ -446,12 +486,12 @@
         <v>3601.44</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>43314</v>
       </c>
       <c r="C3">
-        <v>0.9252</v>
+        <v>0.92520000000000002</v>
       </c>
       <c r="D3">
         <v>-4000</v>
@@ -460,7 +500,7 @@
         <v>4319.07</v>
       </c>
       <c r="G3">
-        <v>1.031</v>
+        <v>1.0309999999999999</v>
       </c>
       <c r="H3">
         <v>-4000</v>
@@ -469,7 +509,7 @@
         <v>3873.92</v>
       </c>
       <c r="K3">
-        <v>0.545</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="L3">
         <v>-6000</v>
@@ -478,7 +518,7 @@
         <v>10995.98</v>
       </c>
       <c r="S3">
-        <v>1.11</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="T3">
         <v>-3000</v>
@@ -487,13 +527,13 @@
         <v>2698.66</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>TODAY()</f>
-        <v>43318</v>
+        <f ca="1">TODAY()</f>
+        <v>43321</v>
       </c>
       <c r="C4">
-        <v>0.9211</v>
+        <v>0.92110000000000003</v>
       </c>
       <c r="D4">
         <f>E4*C4</f>
@@ -504,33 +544,33 @@
         <v>6467.23</v>
       </c>
       <c r="G4">
-        <v>1.019</v>
+        <v>1.0189999999999999</v>
       </c>
       <c r="H4">
         <f>I4*G4</f>
-        <v>5938.660669999999</v>
+        <v>5938.6606699999993</v>
       </c>
       <c r="I4">
         <f>SUM(I2:I3)</f>
         <v>5827.93</v>
       </c>
       <c r="K4">
-        <v>0.538</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="L4">
         <f>M4*K4</f>
-        <v>8852.1982</v>
+        <v>8852.1982000000007</v>
       </c>
       <c r="M4">
         <f>SUM(M2:M3)</f>
-        <v>16453.9</v>
+        <v>16453.900000000001</v>
       </c>
       <c r="O4">
-        <v>0.833</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="P4">
         <f>Q4*O4</f>
-        <v>2999.99952</v>
+        <v>2999.9995199999998</v>
       </c>
       <c r="Q4">
         <f>SUM(Q2:Q3)</f>
@@ -541,73 +581,79 @@
       </c>
       <c r="T4">
         <f>U4*S4</f>
-        <v>2971.22466</v>
+        <v>2971.2246599999999</v>
       </c>
       <c r="U4">
         <f>SUM(U2:U3)</f>
         <v>2698.66</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D5">
         <f>(SUM(D2:D4) )/ -SUM(D2:D3)</f>
-        <v>-0.007172407833333333</v>
+        <v>-7.1724078333333333E-3</v>
       </c>
       <c r="E5">
-        <f>XIRR(D2:D4,A2:A4)</f>
-        <v>-0.20747236683964737</v>
+        <f ca="1">XIRR(D2:D4,A2:A4)</f>
+        <v>-0.16777348406612874</v>
       </c>
       <c r="H5">
         <f>(SUM(H2:H4) )/ -SUM(H2:H3)</f>
-        <v>-0.010223221666666784</v>
+        <v>-1.0223221666666784E-2</v>
       </c>
       <c r="I5">
-        <f>XIRR(H2:H4,A2:A4)</f>
-        <v>-0.28278196975588804</v>
+        <f ca="1">XIRR(H2:H4,A2:A4)</f>
+        <v>-0.23078273460268978</v>
       </c>
       <c r="L5">
         <f>(SUM(L2:L4) )/ -SUM(L2:L3)</f>
-        <v>-0.016422422222222142</v>
+        <v>-1.6422422222222142E-2</v>
       </c>
       <c r="M5">
-        <f>XIRR(L2:L4,A2:A4)</f>
-        <v>-0.41551564261317253</v>
+        <f ca="1">XIRR(L2:L4,A2:A4)</f>
+        <v>-0.34525492265820507</v>
       </c>
       <c r="P5">
         <f>(SUM(P2:P4) )/ -SUM(P2:P3)</f>
-        <v>-1.600000000507862e-7</v>
+        <v>-1.6000000005078619E-7</v>
       </c>
       <c r="Q5">
-        <f>XIRR(P2:P4,A2:A4)</f>
-        <v>-0.0000022441148757934574</v>
+        <f ca="1">XIRR(P2:P4,A2:A4)</f>
+        <v>-2.0116567611694336E-6</v>
       </c>
       <c r="T5">
         <f>(SUM(T2:T4) )/ -SUM(T2:T3)</f>
-        <v>-0.009591780000000048</v>
+        <v>-9.591780000000048E-3</v>
       </c>
       <c r="U5">
-        <f>XIRR(T2:T4,A2:A4)</f>
-        <v>2.9802322387695314e-9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>new data</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
+        <f ca="1">XIRR(T2:T4,A2:A4)</f>
+        <v>2.9802322387695314E-9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U6"/>
+    <ignoredError sqref="A1:U5 E6:U6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A37D344-0F5C-CF47-B4B4-B3A6D0D6BD60}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>43320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>